<commit_message>
Updated crawley neighbourhood areas to better sizing, added Forge Wood area, updated area sizes. Updated Excel table and area graph.
</commit_message>
<xml_diff>
--- a/gis-projects/starter-crawley-map/crawley-data.xlsx
+++ b/gis-projects/starter-crawley-map/crawley-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\personal_projects\data-analysis-project\gis-projects\starter-crawley-map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A6F9BD-D982-4FFF-9065-6F50D775E595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01C37E2-EAFD-4227-AAEB-91AD89B479CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{11A02B39-82FE-4A4C-B0AF-75B70644D236}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{11A02B39-82FE-4A4C-B0AF-75B70644D236}"/>
   </bookViews>
   <sheets>
     <sheet name="Crawley Map" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>area-name</t>
   </si>
@@ -90,21 +90,48 @@
     <t>Northgate</t>
   </si>
   <si>
-    <t>Worth</t>
+    <t>Sum</t>
   </si>
   <si>
-    <t>Town Centre</t>
+    <t>Forge Wood</t>
   </si>
   <si>
-    <t>Sum</t>
+    <r>
+      <t>NOTE: Actual area of Crawley is 44.96km</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -120,7 +147,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -135,19 +162,6 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -208,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -225,9 +239,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -248,11 +259,64 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
         <right/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
@@ -279,59 +343,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color rgb="FF000000"/>
@@ -340,15 +351,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -356,6 +358,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -422,7 +433,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Area in km^2</a:t>
+              <a:t>Area in km</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="30000"/>
+              <a:t>2</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -497,7 +512,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-B631-4CCB-99B4-D2246FE6AE31}"/>
+                <c16:uniqueId val="{00000001-E399-4134-9BC6-1450A4BC4C14}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -516,7 +531,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-B631-4CCB-99B4-D2246FE6AE31}"/>
+                <c16:uniqueId val="{00000003-E399-4134-9BC6-1450A4BC4C14}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -535,7 +550,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-B631-4CCB-99B4-D2246FE6AE31}"/>
+                <c16:uniqueId val="{00000005-E399-4134-9BC6-1450A4BC4C14}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -554,7 +569,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-B631-4CCB-99B4-D2246FE6AE31}"/>
+                <c16:uniqueId val="{00000007-E399-4134-9BC6-1450A4BC4C14}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -573,7 +588,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-B631-4CCB-99B4-D2246FE6AE31}"/>
+                <c16:uniqueId val="{00000009-E399-4134-9BC6-1450A4BC4C14}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -592,7 +607,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000B-B631-4CCB-99B4-D2246FE6AE31}"/>
+                <c16:uniqueId val="{0000000B-E399-4134-9BC6-1450A4BC4C14}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -613,7 +628,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000D-B631-4CCB-99B4-D2246FE6AE31}"/>
+                <c16:uniqueId val="{0000000D-E399-4134-9BC6-1450A4BC4C14}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -634,7 +649,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000F-B631-4CCB-99B4-D2246FE6AE31}"/>
+                <c16:uniqueId val="{0000000F-E399-4134-9BC6-1450A4BC4C14}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -655,7 +670,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000011-B631-4CCB-99B4-D2246FE6AE31}"/>
+                <c16:uniqueId val="{00000011-E399-4134-9BC6-1450A4BC4C14}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -676,7 +691,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000013-B631-4CCB-99B4-D2246FE6AE31}"/>
+                <c16:uniqueId val="{00000013-E399-4134-9BC6-1450A4BC4C14}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -697,7 +712,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000015-B631-4CCB-99B4-D2246FE6AE31}"/>
+                <c16:uniqueId val="{00000015-E399-4134-9BC6-1450A4BC4C14}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -718,7 +733,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000017-B631-4CCB-99B4-D2246FE6AE31}"/>
+                <c16:uniqueId val="{00000017-E399-4134-9BC6-1450A4BC4C14}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -740,7 +755,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000019-B631-4CCB-99B4-D2246FE6AE31}"/>
+                <c16:uniqueId val="{00000019-E399-4134-9BC6-1450A4BC4C14}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -762,29 +777,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000001B-B631-4CCB-99B4-D2246FE6AE31}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="14"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000001D-B631-4CCB-99B4-D2246FE6AE31}"/>
+                <c16:uniqueId val="{0000001B-E399-4134-9BC6-1450A4BC4C14}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -851,59 +844,56 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Neighbourhood Area'!$C$5:$D$19</c15:sqref>
+                    <c15:sqref>'Neighbourhood Area'!$C$5:$D$18</c15:sqref>
                   </c15:fullRef>
                   <c15:levelRef>
-                    <c15:sqref>'Neighbourhood Area'!$C$5:$C$19</c15:sqref>
+                    <c15:sqref>'Neighbourhood Area'!$C$5:$C$18</c15:sqref>
                   </c15:levelRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Neighbourhood Area'!$C$5:$C$19</c:f>
+              <c:f>'Neighbourhood Area'!$C$5:$C$18</c:f>
               <c:strCache>
-                <c:ptCount val="15"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>Town Centre</c:v>
+                  <c:v>Gossops Green</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Worth</c:v>
+                  <c:v>West Green</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Bewbush</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maidenbower</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Southgate</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Three Bridges</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Ifield</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>Northgate</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>Gossops Green</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
+                  <c:v>Furnace Green</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Broadfield</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Tilgate</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>West Green</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Bewbush</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Furnace Green</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Maidenbower</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Southgate</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Three Bridges</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>Ifield</c:v>
+                  <c:v>Pound Hill</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Broadfield</c:v>
+                  <c:v>Forge Wood</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Pound Hill</c:v>
-                </c:pt>
-                <c:pt idx="14">
                   <c:v>Langley Green &amp; Tushmore</c:v>
                 </c:pt>
               </c:strCache>
@@ -911,61 +901,58 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Neighbourhood Area'!$E$5:$E$19</c:f>
+              <c:f>'Neighbourhood Area'!$E$5:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.253</c:v>
+                  <c:v>1.1519999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.57899999999999996</c:v>
+                  <c:v>1.2090000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.95499999999999996</c:v>
+                  <c:v>1.43</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1519999999999999</c:v>
+                  <c:v>1.784</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.181</c:v>
+                  <c:v>1.792</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2050000000000001</c:v>
+                  <c:v>1.804</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.43</c:v>
+                  <c:v>2.3140000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.472</c:v>
+                  <c:v>2.3199999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.784</c:v>
+                  <c:v>2.3940000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.792</c:v>
+                  <c:v>2.492</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.804</c:v>
+                  <c:v>2.66</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.3140000000000001</c:v>
+                  <c:v>3.2469999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.492</c:v>
+                  <c:v>4.9020000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.6739999999999999</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4.9720000000000004</c:v>
+                  <c:v>14.106</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-49CB-430F-BE4A-BB98F8E4EED9}"/>
+              <c16:uniqueId val="{0000001C-E399-4134-9BC6-1450A4BC4C14}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1139,8 +1126,12 @@
                   <a:t>Area (km</a:t>
                 </a:r>
                 <a:r>
+                  <a:rPr lang="en-GB" baseline="30000"/>
+                  <a:t>2</a:t>
+                </a:r>
+                <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t>^2)</a:t>
+                  <a:t>)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB"/>
               </a:p>
@@ -1802,23 +1793,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>181336</xdr:rowOff>
+      <xdr:colOff>23976</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>175261</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5FF4EBF-4CEF-415E-A899-6882A31764D7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F183364-EB03-6172-19F1-BA8B73D36925}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1834,8 +1825,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="6118860" cy="5484856"/>
+          <a:off x="609600" y="182881"/>
+          <a:ext cx="5510376" cy="5478780"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1852,26 +1843,28 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>160020</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>548640</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>533400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD4DDAAD-A09C-7795-DC9F-06B553F3F12E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{540A798B-F3AE-4BCA-88D8-5A71F627D572}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1889,15 +1882,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{764993B1-A42B-4044-909B-04E4928A230F}" name="Table2" displayName="Table2" ref="C4:E20" totalsRowCount="1" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="C4:E19" xr:uid="{764993B1-A42B-4044-909B-04E4928A230F}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C5:E19">
-    <sortCondition ref="E4:E19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{764993B1-A42B-4044-909B-04E4928A230F}" name="Table2" displayName="Table2" ref="C4:E19" totalsRowCount="1" headerRowDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+  <autoFilter ref="C4:E18" xr:uid="{764993B1-A42B-4044-909B-04E4928A230F}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C5:E18">
+    <sortCondition ref="E4:E18"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="2" xr3:uid="{6199CA05-9AD4-4A4D-9F69-7129AF60FB7C}" name="area-name" totalsRowLabel="Sum" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{14A14A14-235C-4FCC-B1B2-7A063AD5BCE9}" name="location" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{A6922492-4382-4F07-A061-B8E4677EDE64}" name="area-size" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{6199CA05-9AD4-4A4D-9F69-7129AF60FB7C}" name="area-name" totalsRowLabel="Sum" dataDxfId="4" totalsRowDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{14A14A14-235C-4FCC-B1B2-7A063AD5BCE9}" name="location" dataDxfId="3" totalsRowDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{A6922492-4382-4F07-A061-B8E4677EDE64}" name="area-size" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2202,8 +2195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A144F6A3-188C-43F0-88C8-12650C910D2D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2215,10 +2208,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85702CCF-1490-41DD-BEB8-C02796F2B8EA}">
-  <dimension ref="C4:E20"/>
+  <dimension ref="C4:F20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2227,196 +2220,192 @@
     <col min="2" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" customWidth="1"/>
+    <col min="6" max="6" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="2">
-        <v>0.253</v>
+      <c r="E5" s="1">
+        <v>1.1519999999999999</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="2">
-        <v>0.57899999999999996</v>
+      <c r="E6" s="1">
+        <v>1.2090000000000001</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="2">
-        <v>0.95499999999999996</v>
+      <c r="E7" s="1">
+        <v>1.43</v>
       </c>
     </row>
-    <row r="8" spans="3:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="2">
-        <v>1.1519999999999999</v>
+      <c r="E8" s="1">
+        <v>1.784</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="2">
-        <v>1.181</v>
+      <c r="E9" s="1">
+        <v>1.792</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="2">
-        <v>1.2050000000000001</v>
+      <c r="E10" s="1">
+        <v>1.804</v>
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C11" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="2">
-        <v>1.43</v>
+      <c r="E11" s="1">
+        <v>2.3140000000000001</v>
       </c>
     </row>
-    <row r="12" spans="3:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="2">
-        <v>1.472</v>
+      <c r="E12" s="1">
+        <v>2.3199999999999998</v>
       </c>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="2">
-        <v>1.784</v>
+      <c r="E13" s="1">
+        <v>2.3940000000000001</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="2">
-        <v>1.792</v>
+      <c r="E14" s="1">
+        <v>2.492</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C15" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="2">
-        <v>1.804</v>
+      <c r="E15" s="1">
+        <v>2.66</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C16" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="2">
-        <v>2.3140000000000001</v>
+      <c r="E16" s="1">
+        <v>3.2469999999999999</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C17" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="2">
-        <v>2.492</v>
+      <c r="E17" s="1">
+        <v>4.9020000000000001</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C18" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="2">
-        <v>2.6739999999999999</v>
+      <c r="E18" s="1">
+        <v>14.106</v>
       </c>
     </row>
-    <row r="19" spans="3:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C19" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="6">
-        <v>4.9720000000000004</v>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5">
+        <f>SUBTOTAL(109,Table2[area-size])</f>
+        <v>43.606000000000002</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C20" s="5" t="s">
+    <row r="20" spans="3:6" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
         <v>19</v>
-      </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="6">
-        <f>SUBTOTAL(109,Table2[area-size])</f>
-        <v>26.059000000000001</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>